<commit_message>
Updated some simper genus outputs
</commit_message>
<xml_diff>
--- a/Simper_Genus/stevia.genus.post_krusk_simper.xlsx
+++ b/Simper_Genus/stevia.genus.post_krusk_simper.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\Simper_Genus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chian\Documents\GitHub\Stevia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96335A86-EB47-4E9B-B865-0E3EA934BCAC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{67BB5BEE-40F1-4BD4-8766-8B0AB83CDB08}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stevia.genus.post_krusk_simper" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="33">
   <si>
     <t>Comparison</t>
   </si>
@@ -70,70 +71,52 @@
     <t>Otu00023</t>
   </si>
   <si>
-    <t>Bacteroidetes - Bacteroidia - Bacteroidales - Bacteroidaceae - Bacteroides</t>
+    <t>Bacteroidetes - Bacteroidia - Bacteroidales - Rikenellaceae - Alistipes</t>
   </si>
   <si>
     <t>Otu00015</t>
   </si>
   <si>
+    <t>Firmicutes - Clostridia - Clostridiales - Lachnospiraceae - Lachnospiraceae_NK4A136_group</t>
+  </si>
+  <si>
     <t>Low Fat_Saccharin</t>
   </si>
   <si>
     <t>Low Fat_Stevia</t>
   </si>
   <si>
-    <t>Tenericutes - Mollicutes - Anaeroplasmatales - Anaeroplasmataceae - Anaeroplasma</t>
-  </si>
-  <si>
     <t>Otu00012</t>
   </si>
   <si>
+    <t>Firmicutes - Clostridia - Clostridiales - Lachnospiraceae - Lachnospiraceae_unclassified</t>
+  </si>
+  <si>
+    <t>Otu00014</t>
+  </si>
+  <si>
+    <t>Firmicutes - Bacilli - Lactobacillales - Streptococcaceae - Lactococcus</t>
+  </si>
+  <si>
+    <t>High Fat_Saccharin</t>
+  </si>
+  <si>
+    <t>Otu00010</t>
+  </si>
+  <si>
     <t>Firmicutes - Clostridia - Clostridiales - Ruminococcaceae - Ruminiclostridium</t>
   </si>
   <si>
-    <t>Otu00014</t>
-  </si>
-  <si>
-    <t>High Fat_Saccharin</t>
-  </si>
-  <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Lachnospiraceae - Lachnospiraceae_unclassified</t>
-  </si>
-  <si>
-    <t>Firmicutes - Bacilli - Lactobacillales - Streptococcaceae - Lactococcus</t>
-  </si>
-  <si>
-    <t>Otu00010</t>
-  </si>
-  <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Lachnospiraceae - Lachnospiraceae_NK4A136_group</t>
-  </si>
-  <si>
     <t>High Fat_Stevia</t>
   </si>
   <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Ruminococcaceae - Oscillibacter</t>
-  </si>
-  <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Clostridiales_vadinBB60_group - Clostridiales_vadinBB60_group_ge</t>
-  </si>
-  <si>
     <t>Otu00018</t>
   </si>
   <si>
     <t>Firmicutes - Bacilli - Lactobacillales - Lactobacillaceae - Lactobacillus</t>
   </si>
   <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Ruminococcaceae - Ruminiclostridium_9</t>
-  </si>
-  <si>
     <t>Saccharin_Stevia</t>
-  </si>
-  <si>
-    <t>Bacteroidetes - Bacteroidia - Bacteroidales - Rikenellaceae - Alistipes</t>
-  </si>
-  <si>
-    <t>Firmicutes - Clostridia - Clostridiales - Ruminococcaceae - Ruminococcaceae_unclassified</t>
   </si>
   <si>
     <t>Male_Female</t>
@@ -279,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,7 +444,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -626,10 +627,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,13 +992,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="88.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="99.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -1028,900 +1034,900 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
-        <v>7.9751723965703E-2</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2">
+        <v>7.9751723999999996E-2</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="1">
-        <v>2.3856345402870999E-4</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2.2265922376012901E-3</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2">
+        <v>2.3856300000000001E-4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>0.106679511</v>
+      </c>
+      <c r="H2">
+        <v>3.8426265000000001E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.5815092999999999E-2</v>
+      </c>
+      <c r="J2">
+        <v>1.0786532E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0.142478201</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1.8940999999999999E-4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>1.8969130000000001E-3</v>
+      </c>
+      <c r="H3">
+        <v>5.818513E-3</v>
+      </c>
+      <c r="I3">
+        <v>0.15343805499999999</v>
+      </c>
+      <c r="J3">
+        <v>0.11177214100000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>7.5243327999999998E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9.5500000000000004E-5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>8.7062914000000005E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.8027219999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.206646304</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>6.0517199999999996E-4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1">
-        <v>0.106679511369612</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3.8426264635317502E-2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1.58150928329817E-2</v>
-      </c>
-      <c r="J2" s="1">
-        <v>1.0786531810485001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.14247820071216499</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="G5">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H5">
+        <v>0.111942318</v>
+      </c>
+      <c r="I5">
+        <v>0.219070502</v>
+      </c>
+      <c r="J5">
+        <v>3.4335400000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>0.20352909799999999</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>7.3444099999999996E-4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.111942318</v>
+      </c>
+      <c r="I6">
+        <v>0.21877064399999999</v>
+      </c>
+      <c r="J6">
+        <v>3.4168054000000003E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>9.7198630999999994E-2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>7.3444099999999996E-4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7">
+        <v>6.4100911999999996E-2</v>
+      </c>
+      <c r="H7">
+        <v>2.8943041999999999E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.17616278199999999</v>
+      </c>
+      <c r="J7">
+        <v>3.8168339000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>8.7406775000000006E-2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>5.3200600000000002E-4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>3.1825777999999999E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.0726954E-2</v>
+      </c>
+      <c r="I8">
+        <v>8.7062914000000005E-2</v>
+      </c>
+      <c r="J8">
+        <v>2.8027219999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>9.7082481999999998E-2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>1.7464749999999999E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>6.1126619999999996E-3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9">
+        <v>0.108325782</v>
+      </c>
+      <c r="H9">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I9">
+        <v>6.2830120000000001E-3</v>
+      </c>
+      <c r="J9">
+        <v>8.0234039999999996E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>0.115731349</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1">
-        <v>1.8940954875338001E-4</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2.2265922376012901E-3</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D10">
+        <v>3.5737569999999999E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.0006519E-2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>1.8969130000000001E-3</v>
+      </c>
+      <c r="H10">
+        <v>5.818513E-3</v>
+      </c>
+      <c r="I10">
+        <v>0.132911325</v>
+      </c>
+      <c r="J10">
+        <v>8.8061366000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>0.17501360799999999</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>3.288614E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.0006519E-2</v>
+      </c>
+      <c r="F11" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="1">
-        <v>1.8969125861471401E-3</v>
-      </c>
-      <c r="H3" s="1">
-        <v>5.8185129323184998E-3</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0.15343805516593201</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0.111772141133741</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1">
-        <v>7.5243327710908997E-2</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2">
-        <v>9.5488256257511201E-5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2.2265922376012901E-3</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G11">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H11">
+        <v>0.111942318</v>
+      </c>
+      <c r="I11">
+        <v>0.275802624</v>
+      </c>
+      <c r="J11">
+        <v>3.5083233999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>8.7447873999999995E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>4.3608420000000002E-3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.1100324E-2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>0.108325782</v>
+      </c>
+      <c r="H12">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I12">
+        <v>1.1503612999999999E-2</v>
+      </c>
+      <c r="J12">
+        <v>2.6562764999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0.10165147500000001</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>7.0766450000000003E-3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.5242004999999999E-2</v>
+      </c>
+      <c r="F13" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>8.7062914046147299E-2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2.8027219940559199E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="G13">
+        <v>0.219070502</v>
+      </c>
+      <c r="H13">
+        <v>3.4335400000000002E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.275802624</v>
+      </c>
+      <c r="J13">
+        <v>3.5083233999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>9.6821675999999995E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>7.0536380000000001E-3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.5242004999999999E-2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0.275802624</v>
+      </c>
+      <c r="H14">
+        <v>3.5083233999999998E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.21877064399999999</v>
+      </c>
+      <c r="J14">
+        <v>3.4168054000000003E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>0.206646304076262</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1">
-        <v>6.0517226253803803E-4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2.9377642391421599E-3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0.45328285954907299</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.11194231809798701</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0.219070502018367</v>
-      </c>
-      <c r="J5" s="1">
-        <v>3.4335399775989997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.20352909806313699</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1">
-        <v>7.3444105978553997E-4</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2.9377642391421599E-3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.45328285954907299</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.11194231809798701</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0.21877064394332399</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3.41680537598123E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1">
-        <v>9.7198630786768006E-2</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7.3444105978553997E-4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.9377642391421599E-3</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1">
-        <v>6.4100912236013996E-2</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2.8943041755505401E-2</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.17616278182011799</v>
-      </c>
-      <c r="J7" s="1">
-        <v>3.8168338508585802E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1">
-        <v>8.7406774772876894E-2</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5.3200550513924998E-4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2.9377642391421599E-3</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="1">
-        <v>3.1825777714928297E-2</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1.07269535915539E-2</v>
-      </c>
-      <c r="I8" s="1">
-        <v>8.7062914046147299E-2</v>
-      </c>
-      <c r="J8" s="1">
-        <v>2.8027219940559199E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1">
-        <v>9.7082481736410001E-2</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B15">
+        <v>8.0130598999999997E-2</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="1">
-        <v>1.7464749096179899E-3</v>
-      </c>
-      <c r="E9" s="1">
-        <v>6.1126621836629803E-3</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.108325782485526</v>
-      </c>
-      <c r="H9" s="1">
-        <v>7.81065956789877E-2</v>
-      </c>
-      <c r="I9" s="1">
-        <v>6.2830123863181798E-3</v>
-      </c>
-      <c r="J9" s="1">
-        <v>8.0234043720339293E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.115731349285302</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3.5737568420889298E-3</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.0006519157849E-2</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1.8969125861471401E-3</v>
-      </c>
-      <c r="H10" s="1">
-        <v>5.8185129323184998E-3</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0.13291132548534301</v>
-      </c>
-      <c r="J10" s="1">
-        <v>8.8061366008365796E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.17501360819612</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3.2886143038479598E-3</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1.0006519157849E-2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.45328285954907299</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.11194231809798701</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.275802623672664</v>
-      </c>
-      <c r="J11" s="1">
-        <v>3.5083233518270501E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1">
-        <v>8.7447873945664001E-2</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1">
-        <v>4.3608415052213004E-3</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.11003238314724E-2</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.108325782485526</v>
-      </c>
-      <c r="H12" s="1">
-        <v>7.81065956789877E-2</v>
-      </c>
-      <c r="I12" s="1">
-        <v>1.15036130788346E-2</v>
-      </c>
-      <c r="J12" s="1">
-        <v>2.6562764876871599E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.10165147459754401</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1">
-        <v>7.0766450105698197E-3</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.5242004638150401E-2</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0.219070502018367</v>
-      </c>
-      <c r="H13" s="1">
-        <v>3.4335399775989997E-2</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0.275802623672664</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3.5083233518270501E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="1">
-        <v>9.6821675666159998E-2</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7.0536378880686002E-3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1.5242004638150401E-2</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0.275802623672664</v>
-      </c>
-      <c r="H14" s="1">
-        <v>3.5083233518270501E-2</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.21877064394332399</v>
-      </c>
-      <c r="J14" s="1">
-        <v>3.41680537598123E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="1">
-        <v>8.0130598593548E-2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.9424156736172399E-2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>3.8848313472344798E-2</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="D15">
+        <v>1.9424157000000001E-2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>3.8848313000000002E-2</v>
+      </c>
+      <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="1">
-        <v>0.108325782485526</v>
-      </c>
-      <c r="H15" s="1">
-        <v>7.81065956789877E-2</v>
-      </c>
-      <c r="I15" s="1">
-        <v>2.9487682290991898E-2</v>
-      </c>
-      <c r="J15" s="1">
-        <v>3.8787015485168698E-2</v>
+      <c r="G15">
+        <v>0.108325782</v>
+      </c>
+      <c r="H15">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I15">
+        <v>2.9487682000000001E-2</v>
+      </c>
+      <c r="J15">
+        <v>3.8787015000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B16">
-        <v>0.18892556092513699</v>
+        <v>0.18892556099999999</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16">
-        <v>8.3264516663550503E-2</v>
+        <v>8.3264516999999996E-2</v>
       </c>
       <c r="E16">
-        <v>0.15542709777196101</v>
+        <v>0.15542709800000001</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G16">
-        <v>0.15343805516593201</v>
+        <v>0.15343805499999999</v>
       </c>
       <c r="H16">
-        <v>0.111772141133741</v>
+        <v>0.11177214100000001</v>
       </c>
       <c r="I16">
-        <v>7.0368073664140399E-2</v>
+        <v>7.0368074000000003E-2</v>
       </c>
       <c r="J16">
-        <v>6.8986188459091199E-2</v>
+        <v>6.8986188000000004E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17">
-        <v>6.7019404828161003E-2</v>
+        <v>6.7019405000000004E-2</v>
       </c>
       <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>0.101876059</v>
+      </c>
+      <c r="E17">
+        <v>0.178283102</v>
+      </c>
+      <c r="F17" t="s">
         <v>27</v>
       </c>
-      <c r="D17">
-        <v>0.10187605853790099</v>
-      </c>
-      <c r="E17">
-        <v>0.178283102441327</v>
-      </c>
-      <c r="F17" t="s">
-        <v>34</v>
-      </c>
       <c r="G17">
-        <v>7.0573395875279402E-2</v>
+        <v>7.0573395999999997E-2</v>
       </c>
       <c r="H17">
-        <v>1.54867919439148E-2</v>
+        <v>1.5486791999999999E-2</v>
       </c>
       <c r="I17">
-        <v>9.8570844277043296E-2</v>
+        <v>9.8570844000000005E-2</v>
       </c>
       <c r="J17">
-        <v>3.8138577431193803E-2</v>
+        <v>3.8138577E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18">
-        <v>8.9571515769091004E-2</v>
+        <v>8.9571516000000004E-2</v>
       </c>
       <c r="C18" t="s">
         <v>21</v>
       </c>
       <c r="D18">
-        <v>0.148914673178766</v>
+        <v>0.148914673</v>
       </c>
       <c r="E18">
-        <v>0.24527122641208501</v>
+        <v>0.24527122600000001</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="G18">
-        <v>0.151861171054822</v>
+        <v>0.15186117099999999</v>
       </c>
       <c r="H18">
-        <v>4.4539163548784601E-2</v>
+        <v>4.4539163999999999E-2</v>
       </c>
       <c r="I18">
-        <v>0.17616278182011799</v>
+        <v>0.17616278199999999</v>
       </c>
       <c r="J18">
-        <v>3.8168338508585802E-2</v>
+        <v>3.8168339000000003E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19">
-        <v>0.17701624035990299</v>
+        <v>0.17701623999999999</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
       <c r="D19">
-        <v>0.177665829328151</v>
+        <v>0.177665829</v>
       </c>
       <c r="E19">
-        <v>0.27636906784379001</v>
+        <v>0.276369068</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G19">
-        <v>0.13291132548534301</v>
+        <v>0.132911325</v>
       </c>
       <c r="H19">
-        <v>8.8061366008365796E-2</v>
+        <v>8.8061366000000002E-2</v>
       </c>
       <c r="I19">
-        <v>7.0368073664140399E-2</v>
+        <v>7.0368074000000003E-2</v>
       </c>
       <c r="J19">
-        <v>6.8986188459091199E-2</v>
+        <v>6.8986188000000004E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B20">
-        <v>7.4623864721416994E-2</v>
+        <v>7.4623864999999998E-2</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
       </c>
       <c r="D20">
-        <v>0.24335410102407201</v>
+        <v>0.24335410099999999</v>
       </c>
       <c r="E20">
-        <v>0.35862709624600098</v>
+        <v>0.35862709599999998</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="G20">
-        <v>4.1690213326899699E-2</v>
+        <v>4.1690212999999997E-2</v>
       </c>
       <c r="H20">
-        <v>7.7085400786791797E-2</v>
+        <v>7.7085400999999998E-2</v>
       </c>
       <c r="I20">
-        <v>4.1488841205418403E-2</v>
+        <v>4.1488840999999999E-2</v>
       </c>
       <c r="J20">
-        <v>4.5821800432886098E-2</v>
+        <v>4.5821800000000003E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B21">
-        <v>0.13311146806756999</v>
+        <v>0.13311146800000001</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
       </c>
       <c r="D21">
-        <v>0.28402141154914801</v>
+        <v>0.28402141199999997</v>
       </c>
       <c r="E21">
-        <v>0.39762997616880702</v>
+        <v>0.397629976</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G21">
-        <v>6.2490586300892402E-2</v>
+        <v>6.2490586000000001E-2</v>
       </c>
       <c r="H21">
-        <v>7.6107375457232895E-2</v>
+        <v>7.6107375000000005E-2</v>
       </c>
       <c r="I21">
-        <v>0.113012643756667</v>
+        <v>0.113012644</v>
       </c>
       <c r="J21">
-        <v>0.110473231350004</v>
+        <v>0.11047323100000001</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B22">
-        <v>8.6227088190171997E-2</v>
+        <v>8.6227087999999993E-2</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
       <c r="D22">
-        <v>0.39297080762895698</v>
+        <v>0.392970808</v>
       </c>
       <c r="E22">
-        <v>0.52396107683861004</v>
+        <v>0.52396107700000005</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G22">
-        <v>0.12902611392331301</v>
+        <v>0.129026114</v>
       </c>
       <c r="H22">
-        <v>6.1745791295262697E-2</v>
+        <v>6.1745791000000001E-2</v>
       </c>
       <c r="I22">
-        <v>0.141878458034216</v>
+        <v>0.14187845800000001</v>
       </c>
       <c r="J22">
-        <v>6.10834927206741E-2</v>
+        <v>6.1083493000000003E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B23">
-        <v>8.7062947327002996E-2</v>
+        <v>8.7062947000000002E-2</v>
       </c>
       <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <v>0.441418327</v>
+      </c>
+      <c r="E23">
+        <v>0.54497414200000005</v>
+      </c>
+      <c r="F23" t="s">
         <v>27</v>
       </c>
-      <c r="D23">
-        <v>0.441418326782055</v>
-      </c>
-      <c r="E23">
-        <v>0.54497414191987703</v>
-      </c>
-      <c r="F23" t="s">
-        <v>37</v>
-      </c>
       <c r="G23">
-        <v>9.5230245652808299E-2</v>
+        <v>9.5230246000000005E-2</v>
       </c>
       <c r="H23">
-        <v>6.4646722100781207E-2</v>
+        <v>6.4646722000000004E-2</v>
       </c>
       <c r="I23">
-        <v>9.8570844277043296E-2</v>
+        <v>9.8570844000000005E-2</v>
       </c>
       <c r="J23">
-        <v>3.8138577431193803E-2</v>
+        <v>3.8138577E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B24">
-        <v>0.15219935447115901</v>
+        <v>0.15219935400000001</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
       </c>
       <c r="D24">
-        <v>0.447657330862756</v>
+        <v>0.44765733099999999</v>
       </c>
       <c r="E24">
-        <v>0.54497414191987703</v>
+        <v>0.54497414200000005</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G24">
-        <v>0.28195333637486503</v>
+        <v>0.281953336</v>
       </c>
       <c r="H24">
-        <v>9.9659884170228502E-2</v>
+        <v>9.9659884000000004E-2</v>
       </c>
       <c r="I24">
-        <v>0.31453843463939102</v>
+        <v>0.31453843500000001</v>
       </c>
       <c r="J24">
-        <v>0.13583627803057699</v>
+        <v>0.135836278</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>8.8345602829958E-2</v>
+        <v>8.8345602999999995E-2</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
       </c>
       <c r="D25">
-        <v>0.56599214819578603</v>
+        <v>0.56599214799999997</v>
       </c>
       <c r="E25">
-        <v>0.66032417289508405</v>
+        <v>0.66032417300000001</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G25">
-        <v>0.151861171054822</v>
+        <v>0.15186117099999999</v>
       </c>
       <c r="H25">
-        <v>4.4539163548784601E-2</v>
+        <v>4.4539163999999999E-2</v>
       </c>
       <c r="I25">
-        <v>0.16213559764678101</v>
+        <v>0.16213559799999999</v>
       </c>
       <c r="J25">
-        <v>5.3762218161235102E-2</v>
+        <v>5.3762218000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26">
-        <v>7.3046940988478998E-2</v>
+        <v>7.3046941000000004E-2</v>
       </c>
       <c r="C26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>0.69110222399999999</v>
+      </c>
+      <c r="E26">
+        <v>0.75418147899999999</v>
+      </c>
+      <c r="F26" t="s">
         <v>27</v>
       </c>
-      <c r="D26">
-        <v>0.69110222384484499</v>
-      </c>
-      <c r="E26">
-        <v>0.75418147854740902</v>
-      </c>
-      <c r="F26" t="s">
-        <v>28</v>
-      </c>
       <c r="G26">
-        <v>7.0573395875279402E-2</v>
+        <v>7.0573395999999997E-2</v>
       </c>
       <c r="H26">
-        <v>1.54867919439148E-2</v>
+        <v>1.5486791999999999E-2</v>
       </c>
       <c r="I26">
-        <v>9.5230245652808299E-2</v>
+        <v>9.5230246000000005E-2</v>
       </c>
       <c r="J26">
-        <v>6.4646722100781207E-2</v>
+        <v>6.4646722000000004E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>7.9529435999999995E-2</v>
+      </c>
+      <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="B27">
-        <v>7.952943592601E-2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
       <c r="D27">
-        <v>0.70031137293687895</v>
+        <v>0.70031137300000001</v>
       </c>
       <c r="E27">
-        <v>0.75418147854740902</v>
+        <v>0.75418147899999999</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G27">
-        <v>2.2798832918654501E-2</v>
+        <v>2.2798833000000001E-2</v>
       </c>
       <c r="H27">
-        <v>3.3964719661722299E-2</v>
+        <v>3.3964719999999997E-2</v>
       </c>
       <c r="I27">
-        <v>3.7508759830069599E-2</v>
+        <v>3.7508760000000002E-2</v>
       </c>
       <c r="J27">
-        <v>6.7124426998006304E-2</v>
+        <v>6.7124427E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28">
-        <v>0.19040173499830901</v>
+        <v>0.19040173499999999</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
       </c>
       <c r="D28">
-        <v>0.75715635203097098</v>
+        <v>0.75715635199999998</v>
       </c>
       <c r="E28">
-        <v>0.78519917988397003</v>
+        <v>0.78519918</v>
       </c>
       <c r="F28" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G28">
-        <v>0.13291132548534301</v>
+        <v>0.132911325</v>
       </c>
       <c r="H28">
-        <v>8.8061366008365796E-2</v>
+        <v>8.8061366000000002E-2</v>
       </c>
       <c r="I28">
-        <v>0.15343805516593201</v>
+        <v>0.15343805499999999</v>
       </c>
       <c r="J28">
-        <v>0.111772141133741</v>
+        <v>0.11177214100000001</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
-        <v>6.3823991389294996E-2</v>
+        <v>6.3823990999999997E-2</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
       </c>
       <c r="D29">
-        <v>0.92334184018093501</v>
+        <v>0.92334183999999997</v>
       </c>
       <c r="E29">
-        <v>0.92334184018093501</v>
+        <v>0.92334183999999997</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G29">
-        <v>0.219070502018367</v>
+        <v>0.219070502</v>
       </c>
       <c r="H29">
-        <v>3.4335399775989997E-2</v>
+        <v>3.4335400000000002E-2</v>
       </c>
       <c r="I29">
-        <v>0.21877064394332399</v>
+        <v>0.21877064399999999</v>
       </c>
       <c r="J29">
-        <v>3.41680537598123E-2</v>
+        <v>3.4168054000000003E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1930,4 +1936,507 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="94.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>0.10165147500000001</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>7.0766450000000003E-3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.5242004999999999E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>0.219070502</v>
+      </c>
+      <c r="H2">
+        <v>3.4335400000000002E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.275802624</v>
+      </c>
+      <c r="J2">
+        <v>3.5083233999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3">
+        <v>7.9751723999999996E-2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.3856300000000001E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.106679511</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3.8426265000000001E-2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.5815092999999999E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.0786532E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.206646304</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6.0517199999999996E-4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.111942318</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.219070502</v>
+      </c>
+      <c r="J4" s="3">
+        <v>3.4335400000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.115731349</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>3.5737569999999999E-3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0006519E-2</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.8969130000000001E-3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>5.818513E-3</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.132911325</v>
+      </c>
+      <c r="J5" s="3">
+        <v>8.8061366000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>8.0130598999999997E-2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.9424157000000001E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3.8848313000000002E-2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.108325782</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.9487682000000001E-2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.8787015000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <v>0.142478201</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1.8940999999999999E-4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.8969130000000001E-3</v>
+      </c>
+      <c r="H7" s="4">
+        <v>5.818513E-3</v>
+      </c>
+      <c r="I7" s="4">
+        <v>0.15343805499999999</v>
+      </c>
+      <c r="J7" s="4">
+        <v>0.11177214100000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4">
+        <v>9.7082481999999998E-2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1.7464749999999999E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6.1126619999999996E-3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0.108325782</v>
+      </c>
+      <c r="H8" s="4">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>6.2830120000000001E-3</v>
+      </c>
+      <c r="J8" s="4">
+        <v>8.0234039999999996E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0.17501360799999999</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3.288614E-3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.0006519E-2</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.111942318</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0.275802624</v>
+      </c>
+      <c r="J9" s="4">
+        <v>3.5083233999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5">
+        <v>7.5243327999999998E-2</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="6">
+        <v>9.5500000000000004E-5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>2.2265919999999999E-3</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>8.7062914000000005E-2</v>
+      </c>
+      <c r="J10" s="5">
+        <v>2.8027219999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.20352909799999999</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="5">
+        <v>7.3444099999999996E-4</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.45328286000000001</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.111942318</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.21877064399999999</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.4168054000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5">
+        <v>9.7198630999999994E-2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5">
+        <v>7.3444099999999996E-4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="5">
+        <v>6.4100911999999996E-2</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2.8943041999999999E-2</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.17616278199999999</v>
+      </c>
+      <c r="J12" s="5">
+        <v>3.8168339000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5">
+        <v>8.7447873999999995E-2</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5">
+        <v>4.3608420000000002E-3</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1.1100324E-2</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.108325782</v>
+      </c>
+      <c r="H13" s="5">
+        <v>7.8106596E-2</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.1503612999999999E-2</v>
+      </c>
+      <c r="J13" s="5">
+        <v>2.6562764999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>8.7406775000000006E-2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>5.3200600000000002E-4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.9377639999999998E-3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>3.1825777999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>1.0726954E-2</v>
+      </c>
+      <c r="I14">
+        <v>8.7062914000000005E-2</v>
+      </c>
+      <c r="J14">
+        <v>2.8027219999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>9.6821675999999995E-2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15">
+        <v>7.0536380000000001E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1.5242004999999999E-2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>0.275802624</v>
+      </c>
+      <c r="H15">
+        <v>3.5083233999999998E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.21877064399999999</v>
+      </c>
+      <c r="J15">
+        <v>3.4168054000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J15">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>